<commit_message>
adjust slides and material for day 3
</commit_message>
<xml_diff>
--- a/_day-three/data-raw/Copenhagen_raw.xlsx
+++ b/_day-three/data-raw/Copenhagen_raw.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\corra\Documents\GitHub\ubep\2023-ecdc-rws\_day-two\data-raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54F29142-E48D-420C-999F-B8CE3CB547C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3665228C-9568-41A3-B704-B88AEC864D65}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1350" yWindow="2600" windowWidth="21600" windowHeight="11720" tabRatio="343" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="24220" windowHeight="15500" tabRatio="343" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Copenhagen_raw" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="906" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="909" uniqueCount="44">
   <si>
     <t>id</t>
   </si>
@@ -147,6 +147,12 @@
   </si>
   <si>
     <t>symptoms</t>
+  </si>
+  <si>
+    <t>??</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
@@ -742,9 +748,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -782,7 +788,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -888,7 +894,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1030,7 +1036,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1040,8 +1046,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AQ401"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1:N1"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1331,8 +1337,8 @@
       <c r="B5" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="C5">
-        <v>18</v>
+      <c r="C5" t="s">
+        <v>42</v>
       </c>
       <c r="D5">
         <v>1</v>
@@ -1493,8 +1499,8 @@
       <c r="C7">
         <v>18</v>
       </c>
-      <c r="D7">
-        <v>1</v>
+      <c r="D7" t="s">
+        <v>43</v>
       </c>
       <c r="E7">
         <v>3</v>
@@ -1611,8 +1617,8 @@
         <v>10</v>
       </c>
       <c r="B8" s="2"/>
-      <c r="C8">
-        <v>15</v>
+      <c r="C8" t="s">
+        <v>42</v>
       </c>
       <c r="D8">
         <v>1</v>

</xml_diff>